<commit_message>
added device create test
</commit_message>
<xml_diff>
--- a/Connected Office Web Application-User Acceptance Testing/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application-User Acceptance Testing/Connected Office Test Data.xlsx
@@ -1359,8 +1359,8 @@
       <x:c r="A11" s="2" t="s">
         <x:v>61</x:v>
       </x:c>
-      <x:c r="B11" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B11" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C11" s="2" t="b">
         <x:v>0</x:v>
@@ -1376,8 +1376,8 @@
       <x:c r="A12" s="2" t="s">
         <x:v>63</x:v>
       </x:c>
-      <x:c r="B12" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B12" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C12" s="2" t="b">
         <x:v>0</x:v>
@@ -1393,8 +1393,8 @@
       <x:c r="A13" s="2" t="s">
         <x:v>65</x:v>
       </x:c>
-      <x:c r="B13" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B13" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C13" s="2" t="b">
         <x:v>0</x:v>
@@ -1410,8 +1410,8 @@
       <x:c r="A14" s="2" t="s">
         <x:v>67</x:v>
       </x:c>
-      <x:c r="B14" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B14" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C14" s="2" t="b">
         <x:v>0</x:v>
@@ -1427,8 +1427,8 @@
       <x:c r="A15" s="2" t="s">
         <x:v>69</x:v>
       </x:c>
-      <x:c r="B15" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B15" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C15" s="2" t="b">
         <x:v>0</x:v>
@@ -1444,8 +1444,8 @@
       <x:c r="A16" s="2" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="B16" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B16" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C16" s="2" t="b">
         <x:v>0</x:v>
@@ -1461,8 +1461,8 @@
       <x:c r="A17" s="2" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="B17" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B17" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C17" s="2" t="b">
         <x:v>0</x:v>
@@ -1478,8 +1478,8 @@
       <x:c r="A18" s="2" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="B18" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B18" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C18" s="2" t="b">
         <x:v>0</x:v>
@@ -1495,8 +1495,8 @@
       <x:c r="A19" s="2" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="B19" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B19" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C19" s="2" t="b">
         <x:v>0</x:v>
@@ -1512,8 +1512,8 @@
       <x:c r="A20" s="2" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="B20" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B20" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C20" s="2" t="b">
         <x:v>0</x:v>
@@ -1529,8 +1529,8 @@
       <x:c r="A21" s="2" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="B21" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B21" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C21" s="2" t="b">
         <x:v>0</x:v>
@@ -1546,8 +1546,8 @@
       <x:c r="A22" s="2" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="B22" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B22" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C22" s="2" t="b">
         <x:v>0</x:v>
@@ -1563,8 +1563,8 @@
       <x:c r="A23" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="B23" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B23" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C23" s="2" t="b">
         <x:v>0</x:v>
@@ -1580,8 +1580,8 @@
       <x:c r="A24" s="2" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="B24" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B24" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C24" s="2" t="b">
         <x:v>0</x:v>

</xml_diff>

<commit_message>
Added device and category test function
</commit_message>
<xml_diff>
--- a/Connected Office Web Application-User Acceptance Testing/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application-User Acceptance Testing/Connected Office Test Data.xlsx
@@ -1365,11 +1365,11 @@
       <x:c r="C11" s="2" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D11" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E11" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D11" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E11" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1382,11 +1382,11 @@
       <x:c r="C12" s="2" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D12" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E12" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D12" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E12" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1399,11 +1399,11 @@
       <x:c r="C13" s="2" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D13" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E13" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D13" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E13" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1416,11 +1416,11 @@
       <x:c r="C14" s="2" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D14" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E14" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D14" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E14" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1433,11 +1433,11 @@
       <x:c r="C15" s="2" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D15" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E15" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D15" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E15" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1450,11 +1450,11 @@
       <x:c r="C16" s="2" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D16" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E16" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D16" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E16" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1467,11 +1467,11 @@
       <x:c r="C17" s="2" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D17" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E17" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D17" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E17" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1484,11 +1484,11 @@
       <x:c r="C18" s="2" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D18" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E18" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D18" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E18" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1501,11 +1501,11 @@
       <x:c r="C19" s="2" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D19" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E19" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D19" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E19" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1518,11 +1518,11 @@
       <x:c r="C20" s="2" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D20" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E20" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D20" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E20" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1535,11 +1535,11 @@
       <x:c r="C21" s="2" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D21" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E21" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D21" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E21" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1552,11 +1552,11 @@
       <x:c r="C22" s="2" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D22" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E22" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D22" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E22" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1569,11 +1569,11 @@
       <x:c r="C23" s="2" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D23" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E23" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D23" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E23" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1586,11 +1586,11 @@
       <x:c r="C24" s="2" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D24" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E24" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D24" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E24" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>